<commit_message>
Atualizado por script em 21-12-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/belgium_jupiler-pro-league_2023-2024.xlsx
+++ b/2023/belgium_jupiler-pro-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V145"/>
+  <dimension ref="A1:V147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Cercle Brugge KSV</t>
+          <t>Eupen</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -2421,38 +2421,38 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Genk</t>
+          <t>Club Brugge KV</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J22" t="n">
-        <v>2.55</v>
+        <v>3.76</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>06/08/2023 16:12</t>
+          <t>06/08/2023 18:42</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>2.52</v>
+        <v>8.35</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>13/08/2023 15:56</t>
+          <t>13/08/2023 15:59</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.75</v>
+        <v>4.19</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>06/08/2023 16:12</t>
+          <t>06/08/2023 18:42</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.74</v>
+        <v>5.47</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -2460,24 +2460,24 @@
         </is>
       </c>
       <c r="R22" t="n">
-        <v>2.49</v>
+        <v>1.85</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>06/08/2023 16:12</t>
+          <t>06/08/2023 18:42</t>
         </is>
       </c>
       <c r="T22" t="n">
-        <v>2.71</v>
+        <v>1.36</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>13/08/2023 15:56</t>
+          <t>13/08/2023 15:59</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/cercle-brugge-genk/SGB3AGMA/</t>
+          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/eupen-club-brugge/lWaC8fiN/</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Eupen</t>
+          <t>Cercle Brugge KSV</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -2513,63 +2513,63 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Club Brugge KV</t>
+          <t>Genk</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
-        <v>3.76</v>
+        <v>2.55</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>06/08/2023 18:42</t>
+          <t>06/08/2023 16:12</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>8.35</v>
+        <v>2.52</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
+          <t>13/08/2023 15:56</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>06/08/2023 16:12</t>
+        </is>
+      </c>
+      <c r="P23" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
           <t>13/08/2023 15:59</t>
         </is>
       </c>
-      <c r="N23" t="n">
-        <v>4.19</v>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>06/08/2023 18:42</t>
-        </is>
-      </c>
-      <c r="P23" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>13/08/2023 15:59</t>
-        </is>
-      </c>
       <c r="R23" t="n">
-        <v>1.85</v>
+        <v>2.49</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>06/08/2023 18:42</t>
+          <t>06/08/2023 16:12</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>1.36</v>
+        <v>2.71</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>13/08/2023 15:59</t>
+          <t>13/08/2023 15:56</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/eupen-club-brugge/lWaC8fiN/</t>
+          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/cercle-brugge-genk/SGB3AGMA/</t>
         </is>
       </c>
     </row>
@@ -3149,71 +3149,71 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Genk</t>
+          <t>Gent</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Charleroi</t>
+          <t>St. Truiden</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30" t="n">
-        <v>1.47</v>
+        <v>1.4</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>13/08/2023 18:42</t>
+          <t>13/08/2023 19:42</t>
         </is>
       </c>
       <c r="L30" t="n">
-        <v>1.59</v>
+        <v>1.52</v>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>20/08/2023 15:53</t>
+          <t>20/08/2023 15:57</t>
         </is>
       </c>
       <c r="N30" t="n">
-        <v>4.85</v>
+        <v>5</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>13/08/2023 18:42</t>
+          <t>13/08/2023 19:42</t>
         </is>
       </c>
       <c r="P30" t="n">
-        <v>4.57</v>
+        <v>4.45</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>20/08/2023 15:53</t>
+          <t>20/08/2023 15:59</t>
         </is>
       </c>
       <c r="R30" t="n">
-        <v>5.52</v>
+        <v>6.31</v>
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>13/08/2023 18:42</t>
+          <t>13/08/2023 19:42</t>
         </is>
       </c>
       <c r="T30" t="n">
-        <v>5.25</v>
+        <v>6.41</v>
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>20/08/2023 15:58</t>
+          <t>20/08/2023 15:59</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/genk-charleroi/xlfRPeMc/</t>
+          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/gent-st-truiden/SxmvNg6G/</t>
         </is>
       </c>
     </row>
@@ -3241,71 +3241,71 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Gent</t>
+          <t>Genk</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>St. Truiden</t>
+          <t>Charleroi</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>1.4</v>
+        <v>1.47</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>13/08/2023 19:42</t>
+          <t>13/08/2023 18:42</t>
         </is>
       </c>
       <c r="L31" t="n">
-        <v>1.52</v>
+        <v>1.59</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>20/08/2023 15:57</t>
+          <t>20/08/2023 15:53</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>5</v>
+        <v>4.85</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>13/08/2023 19:42</t>
+          <t>13/08/2023 18:42</t>
         </is>
       </c>
       <c r="P31" t="n">
-        <v>4.45</v>
+        <v>4.57</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>20/08/2023 15:59</t>
+          <t>20/08/2023 15:53</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>6.31</v>
+        <v>5.52</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>13/08/2023 19:42</t>
+          <t>13/08/2023 18:42</t>
         </is>
       </c>
       <c r="T31" t="n">
-        <v>6.41</v>
+        <v>5.25</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>20/08/2023 15:59</t>
+          <t>20/08/2023 15:58</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/gent-st-truiden/SxmvNg6G/</t>
+          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/genk-charleroi/xlfRPeMc/</t>
         </is>
       </c>
     </row>
@@ -13794,6 +13794,190 @@
       <c r="V145" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/genk-kortrijk/vV3nkR7a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>belgium</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>jupiler-pro-league</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E146" s="2" t="n">
+        <v>45280.77083333334</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Cercle Brugge KSV</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>3</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Kortrijk</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>17/12/2023 19:43</t>
+        </is>
+      </c>
+      <c r="L146" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>20/12/2023 18:29</t>
+        </is>
+      </c>
+      <c r="N146" t="n">
+        <v>5.11</v>
+      </c>
+      <c r="O146" t="inlineStr">
+        <is>
+          <t>17/12/2023 19:43</t>
+        </is>
+      </c>
+      <c r="P146" t="n">
+        <v>5.91</v>
+      </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>20/12/2023 18:29</t>
+        </is>
+      </c>
+      <c r="R146" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="S146" t="inlineStr">
+        <is>
+          <t>17/12/2023 19:43</t>
+        </is>
+      </c>
+      <c r="T146" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="U146" t="inlineStr">
+        <is>
+          <t>20/12/2023 18:29</t>
+        </is>
+      </c>
+      <c r="V146" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/cercle-brugge-kortrijk/823Cx9ui/</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>belgium</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>jupiler-pro-league</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E147" s="2" t="n">
+        <v>45280.86458333334</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>KV Mechelen</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
+        <v>3</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>St. Liege</t>
+        </is>
+      </c>
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>17/12/2023 16:12</t>
+        </is>
+      </c>
+      <c r="L147" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>20/12/2023 20:42</t>
+        </is>
+      </c>
+      <c r="N147" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>17/12/2023 16:12</t>
+        </is>
+      </c>
+      <c r="P147" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>20/12/2023 20:18</t>
+        </is>
+      </c>
+      <c r="R147" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>17/12/2023 16:12</t>
+        </is>
+      </c>
+      <c r="T147" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="U147" t="inlineStr">
+        <is>
+          <t>20/12/2023 20:42</t>
+        </is>
+      </c>
+      <c r="V147" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/kv-mechelen-st-liege/ObgyX49S/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 21-12-2023 20:46
</commit_message>
<xml_diff>
--- a/2023/belgium_jupiler-pro-league_2023-2024.xlsx
+++ b/2023/belgium_jupiler-pro-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V147"/>
+  <dimension ref="A1:V148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13981,6 +13981,98 @@
         </is>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>belgium</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>jupiler-pro-league</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E148" s="2" t="n">
+        <v>45281.86458333334</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Gent</t>
+        </is>
+      </c>
+      <c r="G148" t="n">
+        <v>4</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Leuven</t>
+        </is>
+      </c>
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>17/12/2023 13:42</t>
+        </is>
+      </c>
+      <c r="L148" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>21/12/2023 20:44</t>
+        </is>
+      </c>
+      <c r="N148" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>17/12/2023 13:42</t>
+        </is>
+      </c>
+      <c r="P148" t="n">
+        <v>6.48</v>
+      </c>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>21/12/2023 20:44</t>
+        </is>
+      </c>
+      <c r="R148" t="n">
+        <v>6.76</v>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>17/12/2023 13:42</t>
+        </is>
+      </c>
+      <c r="T148" t="n">
+        <v>10.62</v>
+      </c>
+      <c r="U148" t="inlineStr">
+        <is>
+          <t>21/12/2023 20:44</t>
+        </is>
+      </c>
+      <c r="V148" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/gent-leuven/fJ5OZ6P9/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 22-12-2023 20:45
</commit_message>
<xml_diff>
--- a/2023/belgium_jupiler-pro-league_2023-2024.xlsx
+++ b/2023/belgium_jupiler-pro-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V148"/>
+  <dimension ref="A1:V149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14073,6 +14073,98 @@
         </is>
       </c>
     </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>belgium</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>jupiler-pro-league</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E149" s="2" t="n">
+        <v>45282.86458333334</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>RWDM</t>
+        </is>
+      </c>
+      <c r="G149" t="n">
+        <v>1</v>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Club Brugge KV</t>
+        </is>
+      </c>
+      <c r="I149" t="n">
+        <v>6</v>
+      </c>
+      <c r="J149" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>17/12/2023 13:42</t>
+        </is>
+      </c>
+      <c r="L149" t="n">
+        <v>9.23</v>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>22/12/2023 20:38</t>
+        </is>
+      </c>
+      <c r="N149" t="n">
+        <v>5.12</v>
+      </c>
+      <c r="O149" t="inlineStr">
+        <is>
+          <t>17/12/2023 13:42</t>
+        </is>
+      </c>
+      <c r="P149" t="n">
+        <v>5.72</v>
+      </c>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>22/12/2023 20:42</t>
+        </is>
+      </c>
+      <c r="R149" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>17/12/2023 13:42</t>
+        </is>
+      </c>
+      <c r="T149" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="U149" t="inlineStr">
+        <is>
+          <t>22/12/2023 20:42</t>
+        </is>
+      </c>
+      <c r="V149" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/belgium/jupiler-pro-league/rwd-molenbeek-club-brugge/xreTYQvG/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>